<commit_message>
addElement function partly works for node
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Title</t>
   </si>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t>yoffset</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Binder</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -183,7 +195,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr/>
-  <dimension ref="A1:AT1"/>
+  <dimension ref="A1:AT2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -323,6 +335,29 @@
         <v>43</v>
       </c>
     </row>
+    <row r="2" spans="3:11">
+      <c r="C2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
singleElement function was added to modules
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Title</t>
   </si>
@@ -155,6 +155,120 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Thing 1</t>
+  </si>
+  <si>
+    <t>Thing1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t> node</t>
+  </si>
+  <si>
+    <t>Thing 1-1</t>
+  </si>
+  <si>
+    <t>Thing1-1</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>Thing 1-2</t>
+  </si>
+  <si>
+    <t>Thing1-2</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>Thing 2</t>
+  </si>
+  <si>
+    <t>Thing2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Thing 2-1</t>
+  </si>
+  <si>
+    <t>Thing2-1</t>
+  </si>
+  <si>
+    <t>2-1</t>
+  </si>
+  <si>
+    <t>Thing 2-2</t>
+  </si>
+  <si>
+    <t>Thing2-2</t>
+  </si>
+  <si>
+    <t>2-2</t>
+  </si>
+  <si>
+    <t>Thing 2-3</t>
+  </si>
+  <si>
+    <t>Thing2-3</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>Thing 3</t>
+  </si>
+  <si>
+    <t>Thing3</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t> node actor</t>
+  </si>
+  <si>
+    <t>Thing 3-1</t>
+  </si>
+  <si>
+    <t>Thing3-1</t>
+  </si>
+  <si>
+    <t>3-1</t>
+  </si>
+  <si>
+    <t>Thing 3-2</t>
+  </si>
+  <si>
+    <t>Thing3-2</t>
+  </si>
+  <si>
+    <t>3-2</t>
+  </si>
+  <si>
+    <t>Thing 3-3</t>
+  </si>
+  <si>
+    <t>Thing3-3</t>
+  </si>
+  <si>
+    <t>3-3</t>
+  </si>
+  <si>
+    <t>Thing 3-4</t>
+  </si>
+  <si>
+    <t>Thing3-4</t>
+  </si>
+  <si>
+    <t>3-4</t>
   </si>
 </sst>
 </file>
@@ -195,7 +309,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr/>
-  <dimension ref="A1:AT2"/>
+  <dimension ref="A1:AT14"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -348,14 +462,290 @@
       <c r="F2" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>45</v>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>44</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11">
+      <c r="C3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11">
+      <c r="C4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11">
+      <c r="C5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11">
+      <c r="C6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11">
+      <c r="C7" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11">
+      <c r="C8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11">
+      <c r="C9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11">
+      <c r="C10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11">
+      <c r="C11" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11">
+      <c r="C12" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11">
+      <c r="C13" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11">
+      <c r="C14" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
node convertor sets the unoform
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t>Title</t>
   </si>
@@ -157,18 +157,96 @@
     <t/>
   </si>
   <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>OpenClose</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>fadeOn,0.8</t>
+  </si>
+  <si>
+    <t>fadeOff,0.8</t>
+  </si>
+  <si>
+    <t>fadeOpen,1.2</t>
+  </si>
+  <si>
+    <t>fadeClose,1.2</t>
+  </si>
+  <si>
+    <t>macro1</t>
+  </si>
+  <si>
+    <t>uno</t>
+  </si>
+  <si>
+    <t>vvv</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>-100</t>
+  </si>
+  <si>
     <t>Thing 1</t>
   </si>
   <si>
     <t>Thing1</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t> node</t>
   </si>
   <si>
+    <t>ThingOne</t>
+  </si>
+  <si>
+    <t>the first thing</t>
+  </si>
+  <si>
+    <t>Thing 1-2</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>http://nexial.co</t>
+  </si>
+  <si>
+    <t>Nexial website</t>
+  </si>
+  <si>
+    <t>on=Thing1-2</t>
+  </si>
+  <si>
+    <t>off=Thing1-2</t>
+  </si>
+  <si>
+    <t>open=Thing1-2</t>
+  </si>
+  <si>
+    <t>close=Thing1-2</t>
+  </si>
+  <si>
+    <t>open=Thing1&amp;zoom=1.0&amp;panx=500&amp;pany=500</t>
+  </si>
+  <si>
     <t>Thing 1-1</t>
   </si>
   <si>
@@ -178,9 +256,6 @@
     <t>1-1</t>
   </si>
   <si>
-    <t>Thing 1-2</t>
-  </si>
-  <si>
     <t>Thing1-2</t>
   </si>
   <si>
@@ -235,7 +310,91 @@
     <t> node actor</t>
   </si>
   <si>
+    <t>Thing3-IDOverride</t>
+  </si>
+  <si>
+    <t>Thing 3 Subtitle</t>
+  </si>
+  <si>
     <t>Thing 3-1</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>functon</t>
+  </si>
+  <si>
+    <t>thisHoverFunction=1.0</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>thisClickFunciton=2.0</t>
+  </si>
+  <si>
+    <t>dClickFunction=thisUno</t>
+  </si>
+  <si>
+    <t>Nexial Webstie</t>
+  </si>
+  <si>
+    <t>+++&amp;onURL</t>
+  </si>
+  <si>
+    <t>+++&amp;offURL</t>
+  </si>
+  <si>
+    <t>+++&amp;openURL</t>
+  </si>
+  <si>
+    <t>+++&amp;closeURL</t>
+  </si>
+  <si>
+    <t>fadeOn=1.2</t>
+  </si>
+  <si>
+    <t>fadeOff=0.8</t>
+  </si>
+  <si>
+    <t>drawOpen=1.2</t>
+  </si>
+  <si>
+    <t>drawClose=1.0</t>
+  </si>
+  <si>
+    <t>newStyle</t>
+  </si>
+  <si>
+    <t>+++&amp;on=Thing2</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>50</t>
   </si>
   <si>
     <t>Thing3-1</t>
@@ -449,7 +608,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="3:11">
+    <row r="2" spans="3:46">
       <c r="C2" s="0" t="s">
         <v>44</v>
       </c>
@@ -471,13 +630,73 @@
       <c r="K2" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="S2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT2" s="0" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="3" spans="3:11">
+    <row r="3" spans="3:46">
       <c r="C3" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>44</v>
@@ -489,263 +708,1082 @@
         <v>1</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="K3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA3" s="0" t="s">
         <v>51</v>
       </c>
+      <c r="AB3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE3" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK3" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT3" s="0" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="4" spans="3:11">
+    <row r="4" spans="3:46">
       <c r="C4" s="0" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF4" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="0" t="s">
-        <v>51</v>
+      <c r="AG4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ4" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM4" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN4" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT4" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="5" spans="3:11">
+    <row r="5" spans="3:46">
       <c r="C5" s="0" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H5" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI5" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="0" t="s">
-        <v>51</v>
+      <c r="AJ5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN5" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ5" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR5" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT5" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="6" spans="3:11">
+    <row r="6" spans="3:46">
       <c r="C6" s="0" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN6" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>51</v>
+      <c r="AO6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT6" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="7" spans="3:11">
+    <row r="7" spans="3:46">
       <c r="C7" s="0" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="K7" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA7" s="0" t="s">
         <v>51</v>
       </c>
+      <c r="AF7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM7" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN7" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT7" s="0" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="8" spans="3:11">
+    <row r="8" spans="3:46">
       <c r="C8" s="0" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="K8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="V8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="W8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA8" s="0" t="s">
         <v>51</v>
       </c>
+      <c r="AF8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG8" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH8" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI8" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ8" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM8" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO8" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP8" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ8" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR8" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS8" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT8" s="0" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="9" spans="3:11">
+    <row r="9" spans="3:46">
       <c r="C9" s="0" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="K9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="W9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z9" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA9" s="0" t="s">
         <v>51</v>
       </c>
+      <c r="AF9" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH9" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI9" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ9" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM9" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN9" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ9" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR9" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT9" s="0" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="10" spans="3:11">
+    <row r="10" spans="3:46">
       <c r="C10" s="0" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>73</v>
+        <v>98</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="W10" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y10" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB10" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC10" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD10" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG10" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH10" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI10" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ10" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK10" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL10" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM10" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN10" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO10" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP10" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ10" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR10" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS10" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT10" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="11" spans="3:11">
+    <row r="11" spans="3:46">
       <c r="C11" s="0" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>73</v>
+        <v>98</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="U11" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="V11" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="W11" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z11" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA11" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF11" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG11" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH11" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI11" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ11" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL11" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM11" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN11" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO11" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP11" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ11" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR11" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS11" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT11" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="12" spans="3:11">
+    <row r="12" spans="3:46">
       <c r="C12" s="0" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>73</v>
+        <v>98</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="U12" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="V12" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="W12" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF12" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG12" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH12" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI12" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ12" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL12" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM12" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN12" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO12" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP12" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ12" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS12" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT12" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="13" spans="3:11">
+    <row r="13" spans="3:46">
       <c r="C13" s="0" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>73</v>
+        <v>98</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="T13" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="U13" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="V13" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="W13" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF13" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG13" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH13" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI13" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ13" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL13" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM13" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN13" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO13" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP13" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ13" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS13" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT13" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="14" spans="3:11">
+    <row r="14" spans="3:46">
       <c r="C14" s="0" t="s">
-        <v>83</v>
+        <v>136</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>83</v>
+        <v>136</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>73</v>
+        <v>98</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="T14" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="U14" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="V14" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="W14" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF14" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG14" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH14" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI14" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ14" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL14" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM14" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN14" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO14" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP14" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ14" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS14" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT14" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shortdescription was added to node convertor
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
   <si>
     <t>Title</t>
   </si>
@@ -205,6 +205,9 @@
     <t> node</t>
   </si>
   <si>
+    <t>This the Synopsis for Thing 1</t>
+  </si>
+  <si>
     <t>ThingOne</t>
   </si>
   <si>
@@ -256,6 +259,9 @@
     <t>1-1</t>
   </si>
   <si>
+    <t>This the Synopsis for Thing 1-1</t>
+  </si>
+  <si>
     <t>Thing1-2</t>
   </si>
   <si>
@@ -278,6 +284,9 @@
   </si>
   <si>
     <t>2-1</t>
+  </si>
+  <si>
+    <t>Thing 2 could be Synopsized thusly.</t>
   </si>
   <si>
     <t>Thing 2-2</t>
@@ -696,7 +705,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>44</v>
@@ -710,29 +719,32 @@
       <c r="H3" s="0" t="s">
         <v>61</v>
       </c>
+      <c r="I3" s="0" t="s">
+        <v>64</v>
+      </c>
       <c r="K3" s="0" t="s">
         <v>63</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>61</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="S3" s="0" t="s">
         <v>48</v>
@@ -750,10 +762,10 @@
         <v>48</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z3" s="0" t="s">
         <v>50</v>
@@ -762,16 +774,16 @@
         <v>51</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AC3" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AD3" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AE3" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AF3" s="0" t="s">
         <v>52</v>
@@ -789,7 +801,7 @@
         <v>56</v>
       </c>
       <c r="AK3" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AM3" s="0" t="s">
         <v>57</v>
@@ -818,22 +830,25 @@
     </row>
     <row r="4" spans="3:46">
       <c r="C4" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>61</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>82</v>
       </c>
       <c r="K4" s="0" t="s">
         <v>63</v>
@@ -901,22 +916,22 @@
     </row>
     <row r="5" spans="3:46">
       <c r="C5" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>61</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>63</v>
@@ -984,22 +999,22 @@
     </row>
     <row r="6" spans="3:46">
       <c r="C6" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>61</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>63</v>
@@ -1067,22 +1082,25 @@
     </row>
     <row r="7" spans="3:46">
       <c r="C7" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>63</v>
@@ -1150,22 +1168,22 @@
     </row>
     <row r="8" spans="3:46">
       <c r="C8" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>63</v>
@@ -1233,22 +1251,22 @@
     </row>
     <row r="9" spans="3:46">
       <c r="C9" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K9" s="0" t="s">
         <v>63</v>
@@ -1316,168 +1334,168 @@
     </row>
     <row r="10" spans="3:46">
       <c r="C10" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="M10" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="W10" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y10" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD10" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE10" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AF10" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG10" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH10" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI10" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ10" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK10" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AL10" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM10" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="N10" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="O10" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="P10" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q10" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="R10" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="S10" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="T10" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="U10" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="V10" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="W10" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="X10" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y10" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="Z10" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA10" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB10" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AC10" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD10" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="AE10" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="AF10" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG10" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH10" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="AI10" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="AJ10" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK10" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL10" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="AM10" s="0" t="s">
-        <v>96</v>
-      </c>
       <c r="AN10" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AO10" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AP10" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AQ10" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="AR10" s="0" t="s">
         <v>59</v>
       </c>
       <c r="AS10" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AT10" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="3:46">
       <c r="C11" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H11" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="K11" s="0" t="s">
-        <v>98</v>
-      </c>
       <c r="S11" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Z11" s="0" t="s">
         <v>45</v>
@@ -1486,170 +1504,170 @@
         <v>45</v>
       </c>
       <c r="AF11" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AG11" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AH11" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AI11" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AJ11" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AL11" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AM11" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AN11" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AO11" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AP11" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AQ11" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="AR11" s="0" t="s">
         <v>59</v>
       </c>
       <c r="AS11" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AT11" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="3:46">
       <c r="C12" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H12" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="U12" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="V12" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="W12" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF12" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG12" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH12" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI12" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ12" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL12" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM12" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AN12" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO12" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP12" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ12" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="AR12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS12" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="K12" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="S12" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="T12" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="U12" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="V12" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="W12" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z12" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA12" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF12" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG12" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH12" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="AI12" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="AJ12" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL12" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="AM12" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="AN12" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="AO12" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="AP12" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="AQ12" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR12" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS12" s="0" t="s">
-        <v>127</v>
-      </c>
       <c r="AT12" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="3:46">
       <c r="C13" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Z13" s="0" t="s">
         <v>45</v>
@@ -1658,84 +1676,84 @@
         <v>45</v>
       </c>
       <c r="AF13" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AG13" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AH13" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AI13" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AJ13" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AL13" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AM13" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AN13" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AO13" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AP13" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AQ13" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="AR13" s="0" t="s">
         <v>59</v>
       </c>
       <c r="AS13" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AT13" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="3:46">
       <c r="C14" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="V14" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="W14" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Z14" s="0" t="s">
         <v>45</v>
@@ -1744,46 +1762,46 @@
         <v>45</v>
       </c>
       <c r="AF14" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AG14" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AH14" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AI14" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AJ14" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AL14" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AM14" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AN14" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AO14" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AP14" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AQ14" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="AR14" s="0" t="s">
         <v>59</v>
       </c>
       <c r="AS14" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AT14" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>